<commit_message>
Versión 2 con algoritmo actualizado y nuevas gráficas
</commit_message>
<xml_diff>
--- a/Resultados.xlsx
+++ b/Resultados.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F171"/>
+  <dimension ref="A1:F139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -497,10 +497,10 @@
         <v>4</v>
       </c>
       <c r="C6">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6">
-        <v>9999994</v>
+        <v>9999995</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -517,10 +517,10 @@
         <v>5</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D7">
-        <v>9999991</v>
+        <v>9999994</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -577,10 +577,10 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D10">
-        <v>9999978</v>
+        <v>9999977</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -597,10 +597,10 @@
         <v>9</v>
       </c>
       <c r="C11">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D11">
-        <v>9999973</v>
+        <v>9999975</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -617,10 +617,10 @@
         <v>10</v>
       </c>
       <c r="C12">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D12">
-        <v>9999966</v>
+        <v>9999972</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -637,10 +637,10 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D13">
-        <v>9999958</v>
+        <v>9999966</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -657,10 +657,10 @@
         <v>12</v>
       </c>
       <c r="C14">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D14">
-        <v>9999950</v>
+        <v>9999954</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -677,10 +677,10 @@
         <v>13</v>
       </c>
       <c r="C15">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="D15">
-        <v>9999934</v>
+        <v>9999942</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -697,13 +697,13 @@
         <v>14</v>
       </c>
       <c r="C16">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="D16">
-        <v>9999922</v>
+        <v>9999921</v>
       </c>
       <c r="E16">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F16">
         <v>0</v>
@@ -717,13 +717,13 @@
         <v>15</v>
       </c>
       <c r="C17">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="D17">
-        <v>9999904</v>
+        <v>9999903</v>
       </c>
       <c r="E17">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="F17">
         <v>0</v>
@@ -737,16 +737,16 @@
         <v>16</v>
       </c>
       <c r="C18">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="D18">
-        <v>9999883</v>
+        <v>9999876</v>
       </c>
       <c r="E18">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -757,16 +757,16 @@
         <v>17</v>
       </c>
       <c r="C19">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="D19">
-        <v>9999862</v>
+        <v>9999846</v>
       </c>
       <c r="E19">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F19">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -777,16 +777,16 @@
         <v>18</v>
       </c>
       <c r="C20">
-        <v>167</v>
+        <v>189</v>
       </c>
       <c r="D20">
-        <v>9999824</v>
+        <v>9999808</v>
       </c>
       <c r="E20">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="F20">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -797,16 +797,16 @@
         <v>19</v>
       </c>
       <c r="C21">
-        <v>199</v>
+        <v>233</v>
       </c>
       <c r="D21">
-        <v>9999790</v>
+        <v>9999762</v>
       </c>
       <c r="E21">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -817,16 +817,16 @@
         <v>20</v>
       </c>
       <c r="C22">
-        <v>235</v>
+        <v>306</v>
       </c>
       <c r="D22">
-        <v>9999749</v>
+        <v>9999689</v>
       </c>
       <c r="E22">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="F22">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:6">
@@ -837,16 +837,16 @@
         <v>21</v>
       </c>
       <c r="C23">
-        <v>279</v>
+        <v>385</v>
       </c>
       <c r="D23">
-        <v>9999699</v>
+        <v>9999609</v>
       </c>
       <c r="E23">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="F23">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:6">
@@ -857,16 +857,16 @@
         <v>22</v>
       </c>
       <c r="C24">
-        <v>334</v>
+        <v>499</v>
       </c>
       <c r="D24">
-        <v>9999639</v>
+        <v>9999490</v>
       </c>
       <c r="E24">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="F24">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -877,16 +877,16 @@
         <v>23</v>
       </c>
       <c r="C25">
-        <v>402</v>
+        <v>642</v>
       </c>
       <c r="D25">
-        <v>9999564</v>
+        <v>9999342</v>
       </c>
       <c r="E25">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="F25">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -897,16 +897,16 @@
         <v>24</v>
       </c>
       <c r="C26">
-        <v>470</v>
+        <v>815</v>
       </c>
       <c r="D26">
-        <v>9999488</v>
+        <v>9999162</v>
       </c>
       <c r="E26">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="F26">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -917,16 +917,16 @@
         <v>25</v>
       </c>
       <c r="C27">
-        <v>578</v>
+        <v>1079</v>
       </c>
       <c r="D27">
-        <v>9999372</v>
+        <v>9998896</v>
       </c>
       <c r="E27">
-        <v>45</v>
+        <v>24</v>
       </c>
       <c r="F27">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -937,16 +937,16 @@
         <v>26</v>
       </c>
       <c r="C28">
-        <v>696</v>
+        <v>1370</v>
       </c>
       <c r="D28">
-        <v>9999238</v>
+        <v>9998602</v>
       </c>
       <c r="E28">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="F28">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -957,16 +957,16 @@
         <v>27</v>
       </c>
       <c r="C29">
-        <v>851</v>
+        <v>1790</v>
       </c>
       <c r="D29">
-        <v>9999071</v>
+        <v>9998176</v>
       </c>
       <c r="E29">
-        <v>69</v>
+        <v>31</v>
       </c>
       <c r="F29">
-        <v>9</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -977,16 +977,16 @@
         <v>28</v>
       </c>
       <c r="C30">
-        <v>1045</v>
+        <v>2310</v>
       </c>
       <c r="D30">
-        <v>9998859</v>
+        <v>9997644</v>
       </c>
       <c r="E30">
-        <v>86</v>
+        <v>41</v>
       </c>
       <c r="F30">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -997,16 +997,16 @@
         <v>29</v>
       </c>
       <c r="C31">
-        <v>1246</v>
+        <v>2953</v>
       </c>
       <c r="D31">
-        <v>9998637</v>
+        <v>9996989</v>
       </c>
       <c r="E31">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="F31">
-        <v>12</v>
+        <v>8</v>
       </c>
     </row>
     <row r="32" spans="1:6">
@@ -1017,16 +1017,16 @@
         <v>30</v>
       </c>
       <c r="C32">
-        <v>1503</v>
+        <v>3797</v>
       </c>
       <c r="D32">
-        <v>9998359</v>
+        <v>9996124</v>
       </c>
       <c r="E32">
-        <v>125</v>
+        <v>70</v>
       </c>
       <c r="F32">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1037,16 +1037,16 @@
         <v>31</v>
       </c>
       <c r="C33">
-        <v>1816</v>
+        <v>4826</v>
       </c>
       <c r="D33">
-        <v>9998008</v>
+        <v>9995077</v>
       </c>
       <c r="E33">
-        <v>160</v>
+        <v>87</v>
       </c>
       <c r="F33">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1057,16 +1057,16 @@
         <v>32</v>
       </c>
       <c r="C34">
-        <v>2204</v>
+        <v>6156</v>
       </c>
       <c r="D34">
-        <v>9997586</v>
+        <v>9993720</v>
       </c>
       <c r="E34">
-        <v>194</v>
+        <v>113</v>
       </c>
       <c r="F34">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="35" spans="1:6">
@@ -1077,16 +1077,16 @@
         <v>33</v>
       </c>
       <c r="C35">
-        <v>2715</v>
+        <v>7889</v>
       </c>
       <c r="D35">
-        <v>9997034</v>
+        <v>9991957</v>
       </c>
       <c r="E35">
-        <v>231</v>
+        <v>140</v>
       </c>
       <c r="F35">
-        <v>20</v>
+        <v>14</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1097,16 +1097,16 @@
         <v>34</v>
       </c>
       <c r="C36">
-        <v>3310</v>
+        <v>10186</v>
       </c>
       <c r="D36">
-        <v>9996389</v>
+        <v>9989622</v>
       </c>
       <c r="E36">
-        <v>277</v>
+        <v>174</v>
       </c>
       <c r="F36">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -1117,16 +1117,16 @@
         <v>35</v>
       </c>
       <c r="C37">
-        <v>4015</v>
+        <v>13097</v>
       </c>
       <c r="D37">
-        <v>9995624</v>
+        <v>9986665</v>
       </c>
       <c r="E37">
-        <v>335</v>
+        <v>215</v>
       </c>
       <c r="F37">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -1137,16 +1137,16 @@
         <v>36</v>
       </c>
       <c r="C38">
-        <v>4907</v>
+        <v>16764</v>
       </c>
       <c r="D38">
-        <v>9994657</v>
+        <v>9982925</v>
       </c>
       <c r="E38">
-        <v>406</v>
+        <v>282</v>
       </c>
       <c r="F38">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:6">
@@ -1157,16 +1157,16 @@
         <v>37</v>
       </c>
       <c r="C39">
-        <v>5992</v>
+        <v>21506</v>
       </c>
       <c r="D39">
-        <v>9993496</v>
+        <v>9978103</v>
       </c>
       <c r="E39">
-        <v>480</v>
+        <v>353</v>
       </c>
       <c r="F39">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="1:6">
@@ -1177,16 +1177,16 @@
         <v>38</v>
       </c>
       <c r="C40">
-        <v>7282</v>
+        <v>27590</v>
       </c>
       <c r="D40">
-        <v>9992090</v>
+        <v>9971900</v>
       </c>
       <c r="E40">
-        <v>591</v>
+        <v>462</v>
       </c>
       <c r="F40">
-        <v>37</v>
+        <v>48</v>
       </c>
     </row>
     <row r="41" spans="1:6">
@@ -1197,16 +1197,16 @@
         <v>39</v>
       </c>
       <c r="C41">
-        <v>8793</v>
+        <v>35575</v>
       </c>
       <c r="D41">
-        <v>9990445</v>
+        <v>9963767</v>
       </c>
       <c r="E41">
-        <v>717</v>
+        <v>595</v>
       </c>
       <c r="F41">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -1217,16 +1217,16 @@
         <v>40</v>
       </c>
       <c r="C42">
-        <v>10654</v>
+        <v>45637</v>
       </c>
       <c r="D42">
-        <v>9988417</v>
+        <v>9953525</v>
       </c>
       <c r="E42">
-        <v>878</v>
+        <v>756</v>
       </c>
       <c r="F42">
-        <v>51</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:6">
@@ -1237,16 +1237,16 @@
         <v>41</v>
       </c>
       <c r="C43">
-        <v>13002</v>
+        <v>58639</v>
       </c>
       <c r="D43">
-        <v>9985857</v>
+        <v>9940257</v>
       </c>
       <c r="E43">
-        <v>1074</v>
+        <v>992</v>
       </c>
       <c r="F43">
-        <v>67</v>
+        <v>112</v>
       </c>
     </row>
     <row r="44" spans="1:6">
@@ -1257,16 +1257,16 @@
         <v>42</v>
       </c>
       <c r="C44">
-        <v>15731</v>
+        <v>75354</v>
       </c>
       <c r="D44">
-        <v>9982906</v>
+        <v>9923248</v>
       </c>
       <c r="E44">
-        <v>1273</v>
+        <v>1261</v>
       </c>
       <c r="F44">
-        <v>90</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:6">
@@ -1277,16 +1277,16 @@
         <v>43</v>
       </c>
       <c r="C45">
-        <v>19109</v>
+        <v>96332</v>
       </c>
       <c r="D45">
-        <v>9979250</v>
+        <v>9901844</v>
       </c>
       <c r="E45">
-        <v>1541</v>
+        <v>1649</v>
       </c>
       <c r="F45">
-        <v>100</v>
+        <v>175</v>
       </c>
     </row>
     <row r="46" spans="1:6">
@@ -1297,16 +1297,16 @@
         <v>44</v>
       </c>
       <c r="C46">
-        <v>23119</v>
+        <v>123470</v>
       </c>
       <c r="D46">
-        <v>9974889</v>
+        <v>9874174</v>
       </c>
       <c r="E46">
-        <v>1875</v>
+        <v>2127</v>
       </c>
       <c r="F46">
-        <v>117</v>
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:6">
@@ -1317,16 +1317,16 @@
         <v>45</v>
       </c>
       <c r="C47">
-        <v>27936</v>
+        <v>157801</v>
       </c>
       <c r="D47">
-        <v>9969650</v>
+        <v>9839188</v>
       </c>
       <c r="E47">
-        <v>2273</v>
+        <v>2709</v>
       </c>
       <c r="F47">
-        <v>141</v>
+        <v>302</v>
       </c>
     </row>
     <row r="48" spans="1:6">
@@ -1337,16 +1337,16 @@
         <v>46</v>
       </c>
       <c r="C48">
-        <v>33796</v>
+        <v>201330</v>
       </c>
       <c r="D48">
-        <v>9963238</v>
+        <v>9794794</v>
       </c>
       <c r="E48">
-        <v>2799</v>
+        <v>3476</v>
       </c>
       <c r="F48">
-        <v>167</v>
+        <v>400</v>
       </c>
     </row>
     <row r="49" spans="1:6">
@@ -1357,16 +1357,16 @@
         <v>47</v>
       </c>
       <c r="C49">
-        <v>40814</v>
+        <v>256760</v>
       </c>
       <c r="D49">
-        <v>9955575</v>
+        <v>9738317</v>
       </c>
       <c r="E49">
-        <v>3413</v>
+        <v>4428</v>
       </c>
       <c r="F49">
-        <v>198</v>
+        <v>495</v>
       </c>
     </row>
     <row r="50" spans="1:6">
@@ -1377,16 +1377,16 @@
         <v>48</v>
       </c>
       <c r="C50">
-        <v>49401</v>
+        <v>326323</v>
       </c>
       <c r="D50">
-        <v>9946223</v>
+        <v>9667397</v>
       </c>
       <c r="E50">
-        <v>4145</v>
+        <v>5640</v>
       </c>
       <c r="F50">
-        <v>231</v>
+        <v>640</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -1397,16 +1397,16 @@
         <v>49</v>
       </c>
       <c r="C51">
-        <v>59789</v>
+        <v>413589</v>
       </c>
       <c r="D51">
-        <v>9934868</v>
+        <v>9578368</v>
       </c>
       <c r="E51">
-        <v>5063</v>
+        <v>7246</v>
       </c>
       <c r="F51">
-        <v>280</v>
+        <v>797</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -1417,16 +1417,16 @@
         <v>50</v>
       </c>
       <c r="C52">
-        <v>71992</v>
+        <v>522049</v>
       </c>
       <c r="D52">
-        <v>9921504</v>
+        <v>9467573</v>
       </c>
       <c r="E52">
-        <v>6160</v>
+        <v>9323</v>
       </c>
       <c r="F52">
-        <v>344</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="53" spans="1:6">
@@ -1437,16 +1437,16 @@
         <v>51</v>
       </c>
       <c r="C53">
-        <v>86892</v>
+        <v>655858</v>
       </c>
       <c r="D53">
-        <v>9905198</v>
+        <v>9330807</v>
       </c>
       <c r="E53">
-        <v>7489</v>
+        <v>11963</v>
       </c>
       <c r="F53">
-        <v>421</v>
+        <v>1372</v>
       </c>
     </row>
     <row r="54" spans="1:6">
@@ -1457,16 +1457,16 @@
         <v>52</v>
       </c>
       <c r="C54">
-        <v>104829</v>
+        <v>819792</v>
       </c>
       <c r="D54">
-        <v>9885616</v>
+        <v>9163133</v>
       </c>
       <c r="E54">
-        <v>9041</v>
+        <v>15365</v>
       </c>
       <c r="F54">
-        <v>514</v>
+        <v>1710</v>
       </c>
     </row>
     <row r="55" spans="1:6">
@@ -1477,16 +1477,16 @@
         <v>53</v>
       </c>
       <c r="C55">
-        <v>126514</v>
+        <v>1017559</v>
       </c>
       <c r="D55">
-        <v>9861903</v>
+        <v>8960544</v>
       </c>
       <c r="E55">
-        <v>10965</v>
+        <v>19713</v>
       </c>
       <c r="F55">
-        <v>618</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -1497,16 +1497,16 @@
         <v>54</v>
       </c>
       <c r="C56">
-        <v>152580</v>
+        <v>1252822</v>
       </c>
       <c r="D56">
-        <v>9833277</v>
+        <v>8719078</v>
       </c>
       <c r="E56">
-        <v>13407</v>
+        <v>25308</v>
       </c>
       <c r="F56">
-        <v>736</v>
+        <v>2792</v>
       </c>
     </row>
     <row r="57" spans="1:6">
@@ -1517,16 +1517,16 @@
         <v>55</v>
       </c>
       <c r="C57">
-        <v>183820</v>
+        <v>1527055</v>
       </c>
       <c r="D57">
-        <v>9799086</v>
+        <v>8436712</v>
       </c>
       <c r="E57">
-        <v>16203</v>
+        <v>32657</v>
       </c>
       <c r="F57">
-        <v>891</v>
+        <v>3576</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -1537,16 +1537,16 @@
         <v>56</v>
       </c>
       <c r="C58">
-        <v>221510</v>
+        <v>1840420</v>
       </c>
       <c r="D58">
-        <v>9757740</v>
+        <v>8113105</v>
       </c>
       <c r="E58">
-        <v>19660</v>
+        <v>41879</v>
       </c>
       <c r="F58">
-        <v>1090</v>
+        <v>4596</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -1557,16 +1557,16 @@
         <v>57</v>
       </c>
       <c r="C59">
-        <v>266330</v>
+        <v>2188474</v>
       </c>
       <c r="D59">
-        <v>9708559</v>
+        <v>7751783</v>
       </c>
       <c r="E59">
-        <v>23768</v>
+        <v>53834</v>
       </c>
       <c r="F59">
-        <v>1343</v>
+        <v>5909</v>
       </c>
     </row>
     <row r="60" spans="1:6">
@@ -1577,16 +1577,16 @@
         <v>58</v>
       </c>
       <c r="C60">
-        <v>320182</v>
+        <v>2563524</v>
       </c>
       <c r="D60">
-        <v>9649468</v>
+        <v>7359724</v>
       </c>
       <c r="E60">
-        <v>28732</v>
+        <v>69194</v>
       </c>
       <c r="F60">
-        <v>1618</v>
+        <v>7558</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -1597,16 +1597,16 @@
         <v>59</v>
       </c>
       <c r="C61">
-        <v>383930</v>
+        <v>2954632</v>
       </c>
       <c r="D61">
-        <v>9579308</v>
+        <v>6947212</v>
       </c>
       <c r="E61">
-        <v>34817</v>
+        <v>88476</v>
       </c>
       <c r="F61">
-        <v>1945</v>
+        <v>9680</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -1617,16 +1617,16 @@
         <v>60</v>
       </c>
       <c r="C62">
-        <v>459632</v>
+        <v>3347286</v>
       </c>
       <c r="D62">
-        <v>9495943</v>
+        <v>6526888</v>
       </c>
       <c r="E62">
-        <v>42125</v>
+        <v>113383</v>
       </c>
       <c r="F62">
-        <v>2300</v>
+        <v>12443</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -1637,16 +1637,16 @@
         <v>61</v>
       </c>
       <c r="C63">
-        <v>549180</v>
+        <v>3725259</v>
       </c>
       <c r="D63">
-        <v>9397043</v>
+        <v>6113929</v>
       </c>
       <c r="E63">
-        <v>50986</v>
+        <v>144912</v>
       </c>
       <c r="F63">
-        <v>2791</v>
+        <v>15900</v>
       </c>
     </row>
     <row r="64" spans="1:6">
@@ -1657,16 +1657,16 @@
         <v>62</v>
       </c>
       <c r="C64">
-        <v>654934</v>
+        <v>4072429</v>
       </c>
       <c r="D64">
-        <v>9279934</v>
+        <v>5722365</v>
       </c>
       <c r="E64">
-        <v>61743</v>
+        <v>184733</v>
       </c>
       <c r="F64">
-        <v>3389</v>
+        <v>20473</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -1677,16 +1677,16 @@
         <v>63</v>
       </c>
       <c r="C65">
-        <v>779606</v>
+        <v>4375052</v>
       </c>
       <c r="D65">
-        <v>9141898</v>
+        <v>5363265</v>
       </c>
       <c r="E65">
-        <v>74468</v>
+        <v>235620</v>
       </c>
       <c r="F65">
-        <v>4028</v>
+        <v>26063</v>
       </c>
     </row>
     <row r="66" spans="1:6">
@@ -1697,16 +1697,16 @@
         <v>64</v>
       </c>
       <c r="C66">
-        <v>923932</v>
+        <v>4624084</v>
       </c>
       <c r="D66">
-        <v>8981266</v>
+        <v>5043313</v>
       </c>
       <c r="E66">
-        <v>89951</v>
+        <v>299362</v>
       </c>
       <c r="F66">
-        <v>4851</v>
+        <v>33241</v>
       </c>
     </row>
     <row r="67" spans="1:6">
@@ -1717,16 +1717,16 @@
         <v>65</v>
       </c>
       <c r="C67">
-        <v>1090816</v>
+        <v>4810829</v>
       </c>
       <c r="D67">
-        <v>8794800</v>
+        <v>4767539</v>
       </c>
       <c r="E67">
-        <v>108549</v>
+        <v>379409</v>
       </c>
       <c r="F67">
-        <v>5835</v>
+        <v>42223</v>
       </c>
     </row>
     <row r="68" spans="1:6">
@@ -1737,16 +1737,16 @@
         <v>66</v>
       </c>
       <c r="C68">
-        <v>1282538</v>
+        <v>4932280</v>
       </c>
       <c r="D68">
-        <v>8579365</v>
+        <v>4535293</v>
       </c>
       <c r="E68">
-        <v>131079</v>
+        <v>479116</v>
       </c>
       <c r="F68">
-        <v>7018</v>
+        <v>53311</v>
       </c>
     </row>
     <row r="69" spans="1:6">
@@ -1757,16 +1757,16 @@
         <v>67</v>
       </c>
       <c r="C69">
-        <v>1499316</v>
+        <v>4989186</v>
       </c>
       <c r="D69">
-        <v>8333961</v>
+        <v>4341621</v>
       </c>
       <c r="E69">
-        <v>158250</v>
+        <v>602136</v>
       </c>
       <c r="F69">
-        <v>8473</v>
+        <v>67057</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -1777,16 +1777,16 @@
         <v>68</v>
       </c>
       <c r="C70">
-        <v>1742636</v>
+        <v>4980381</v>
       </c>
       <c r="D70">
-        <v>8056450</v>
+        <v>4182752</v>
       </c>
       <c r="E70">
-        <v>190680</v>
+        <v>753055</v>
       </c>
       <c r="F70">
-        <v>10234</v>
+        <v>83812</v>
       </c>
     </row>
     <row r="71" spans="1:6">
@@ -1797,16 +1797,16 @@
         <v>69</v>
       </c>
       <c r="C71">
-        <v>2011917</v>
+        <v>4906790</v>
       </c>
       <c r="D71">
-        <v>7745823</v>
+        <v>4053754</v>
       </c>
       <c r="E71">
-        <v>229926</v>
+        <v>935542</v>
       </c>
       <c r="F71">
-        <v>12334</v>
+        <v>103914</v>
       </c>
     </row>
     <row r="72" spans="1:6">
@@ -1817,16 +1817,16 @@
         <v>70</v>
       </c>
       <c r="C72">
-        <v>2305512</v>
+        <v>4769088</v>
       </c>
       <c r="D72">
-        <v>7403047</v>
+        <v>3949990</v>
       </c>
       <c r="E72">
-        <v>276694</v>
+        <v>1152927</v>
       </c>
       <c r="F72">
-        <v>14747</v>
+        <v>127995</v>
       </c>
     </row>
     <row r="73" spans="1:6">
@@ -1837,16 +1837,16 @@
         <v>71</v>
       </c>
       <c r="C73">
-        <v>2617960</v>
+        <v>4570254</v>
       </c>
       <c r="D73">
-        <v>7031508</v>
+        <v>3866458</v>
       </c>
       <c r="E73">
-        <v>332851</v>
+        <v>1407093</v>
       </c>
       <c r="F73">
-        <v>17681</v>
+        <v>156195</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -1857,16 +1857,16 @@
         <v>72</v>
       </c>
       <c r="C74">
-        <v>2946382</v>
+        <v>4313624</v>
       </c>
       <c r="D74">
-        <v>6632926</v>
+        <v>3799481</v>
       </c>
       <c r="E74">
-        <v>399492</v>
+        <v>1698419</v>
       </c>
       <c r="F74">
-        <v>21200</v>
+        <v>188476</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -1877,16 +1877,16 @@
         <v>73</v>
       </c>
       <c r="C75">
-        <v>3281726</v>
+        <v>4005679</v>
       </c>
       <c r="D75">
-        <v>6214217</v>
+        <v>3746104</v>
       </c>
       <c r="E75">
-        <v>478604</v>
+        <v>2023825</v>
       </c>
       <c r="F75">
-        <v>25453</v>
+        <v>224392</v>
       </c>
     </row>
     <row r="76" spans="1:6">
@@ -1897,16 +1897,16 @@
         <v>74</v>
       </c>
       <c r="C76">
-        <v>3614516</v>
+        <v>3656433</v>
       </c>
       <c r="D76">
-        <v>5782527</v>
+        <v>3703291</v>
       </c>
       <c r="E76">
-        <v>572647</v>
+        <v>2376816</v>
       </c>
       <c r="F76">
-        <v>30310</v>
+        <v>263460</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -1917,16 +1917,16 @@
         <v>75</v>
       </c>
       <c r="C77">
-        <v>3934481</v>
+        <v>3278315</v>
       </c>
       <c r="D77">
-        <v>5345453</v>
+        <v>3668897</v>
       </c>
       <c r="E77">
-        <v>683824</v>
+        <v>2748275</v>
       </c>
       <c r="F77">
-        <v>36242</v>
+        <v>304513</v>
       </c>
     </row>
     <row r="78" spans="1:6">
@@ -1937,16 +1937,16 @@
         <v>76</v>
       </c>
       <c r="C78">
-        <v>4229570</v>
+        <v>2885256</v>
       </c>
       <c r="D78">
-        <v>4912328</v>
+        <v>3641632</v>
       </c>
       <c r="E78">
-        <v>815131</v>
+        <v>3126295</v>
       </c>
       <c r="F78">
-        <v>42971</v>
+        <v>346817</v>
       </c>
     </row>
     <row r="79" spans="1:6">
@@ -1957,16 +1957,16 @@
         <v>77</v>
       </c>
       <c r="C79">
-        <v>4492071</v>
+        <v>2493953</v>
       </c>
       <c r="D79">
-        <v>4489195</v>
+        <v>3619976</v>
       </c>
       <c r="E79">
-        <v>967601</v>
+        <v>3497949</v>
       </c>
       <c r="F79">
-        <v>51133</v>
+        <v>388122</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -1977,16 +1977,16 @@
         <v>78</v>
       </c>
       <c r="C80">
-        <v>4709317</v>
+        <v>2119850</v>
       </c>
       <c r="D80">
-        <v>4085483</v>
+        <v>3602515</v>
       </c>
       <c r="E80">
-        <v>1144801</v>
+        <v>3850095</v>
       </c>
       <c r="F80">
-        <v>60399</v>
+        <v>427540</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -1997,16 +1997,16 @@
         <v>79</v>
       </c>
       <c r="C81">
-        <v>4872467</v>
+        <v>1774420</v>
       </c>
       <c r="D81">
-        <v>3706898</v>
+        <v>3588845</v>
       </c>
       <c r="E81">
-        <v>1349386</v>
+        <v>4172928</v>
       </c>
       <c r="F81">
-        <v>71249</v>
+        <v>463807</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2017,16 +2017,16 @@
         <v>80</v>
       </c>
       <c r="C82">
-        <v>4976797</v>
+        <v>1465285</v>
       </c>
       <c r="D82">
-        <v>3357164</v>
+        <v>3578028</v>
       </c>
       <c r="E82">
-        <v>1582477</v>
+        <v>4461088</v>
       </c>
       <c r="F82">
-        <v>83562</v>
+        <v>495599</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2037,16 +2037,16 @@
         <v>81</v>
       </c>
       <c r="C83">
-        <v>5017349</v>
+        <v>1197922</v>
       </c>
       <c r="D83">
-        <v>3039101</v>
+        <v>3569617</v>
       </c>
       <c r="E83">
-        <v>1845898</v>
+        <v>4709274</v>
       </c>
       <c r="F83">
-        <v>97652</v>
+        <v>523187</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2057,16 +2057,16 @@
         <v>82</v>
       </c>
       <c r="C84">
-        <v>4991030</v>
+        <v>972415</v>
       </c>
       <c r="D84">
-        <v>2754793</v>
+        <v>3562878</v>
       </c>
       <c r="E84">
-        <v>2140944</v>
+        <v>4918071</v>
       </c>
       <c r="F84">
-        <v>113233</v>
+        <v>546636</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2077,16 +2077,16 @@
         <v>83</v>
       </c>
       <c r="C85">
-        <v>4900229</v>
+        <v>783822</v>
       </c>
       <c r="D85">
-        <v>2502818</v>
+        <v>3557799</v>
       </c>
       <c r="E85">
-        <v>2466669</v>
+        <v>5092467</v>
       </c>
       <c r="F85">
-        <v>130284</v>
+        <v>565912</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2097,16 +2097,16 @@
         <v>84</v>
       </c>
       <c r="C86">
-        <v>4748181</v>
+        <v>629029</v>
       </c>
       <c r="D86">
-        <v>2283327</v>
+        <v>3553723</v>
       </c>
       <c r="E86">
-        <v>2819545</v>
+        <v>5235633</v>
       </c>
       <c r="F86">
-        <v>148947</v>
+        <v>581615</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2117,16 +2117,16 @@
         <v>85</v>
       </c>
       <c r="C87">
-        <v>4540056</v>
+        <v>503262</v>
       </c>
       <c r="D87">
-        <v>2092870</v>
+        <v>3550492</v>
       </c>
       <c r="E87">
-        <v>3198205</v>
+        <v>5351836</v>
       </c>
       <c r="F87">
-        <v>168869</v>
+        <v>594410</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2137,16 +2137,16 @@
         <v>86</v>
       </c>
       <c r="C88">
-        <v>4285303</v>
+        <v>402065</v>
       </c>
       <c r="D88">
-        <v>1928914</v>
+        <v>3547925</v>
       </c>
       <c r="E88">
-        <v>3595806</v>
+        <v>5445135</v>
       </c>
       <c r="F88">
-        <v>189977</v>
+        <v>604875</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2157,16 +2157,16 @@
         <v>87</v>
       </c>
       <c r="C89">
-        <v>3994200</v>
+        <v>320544</v>
       </c>
       <c r="D89">
-        <v>1788327</v>
+        <v>3545914</v>
       </c>
       <c r="E89">
-        <v>4006058</v>
+        <v>5520353</v>
       </c>
       <c r="F89">
-        <v>211415</v>
+        <v>613189</v>
       </c>
     </row>
     <row r="90" spans="1:6">
@@ -2177,16 +2177,16 @@
         <v>88</v>
       </c>
       <c r="C90">
-        <v>3676059</v>
+        <v>255158</v>
       </c>
       <c r="D90">
-        <v>1669394</v>
+        <v>3544323</v>
       </c>
       <c r="E90">
-        <v>4421243</v>
+        <v>5580475</v>
       </c>
       <c r="F90">
-        <v>233304</v>
+        <v>620044</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -2197,16 +2197,16 @@
         <v>89</v>
       </c>
       <c r="C91">
-        <v>3344049</v>
+        <v>203021</v>
       </c>
       <c r="D91">
-        <v>1568279</v>
+        <v>3543083</v>
       </c>
       <c r="E91">
-        <v>4832508</v>
+        <v>5628514</v>
       </c>
       <c r="F91">
-        <v>255164</v>
+        <v>625382</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -2217,16 +2217,16 @@
         <v>90</v>
       </c>
       <c r="C92">
-        <v>3006107</v>
+        <v>161207</v>
       </c>
       <c r="D92">
-        <v>1483088</v>
+        <v>3542084</v>
       </c>
       <c r="E92">
-        <v>5234761</v>
+        <v>5667012</v>
       </c>
       <c r="F92">
-        <v>276044</v>
+        <v>629697</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -2237,16 +2237,16 @@
         <v>91</v>
       </c>
       <c r="C93">
-        <v>2673305</v>
+        <v>127547</v>
       </c>
       <c r="D93">
-        <v>1412178</v>
+        <v>3541350</v>
       </c>
       <c r="E93">
-        <v>5618236</v>
+        <v>5697963</v>
       </c>
       <c r="F93">
-        <v>296281</v>
+        <v>633140</v>
       </c>
     </row>
     <row r="94" spans="1:6">
@@ -2257,16 +2257,16 @@
         <v>92</v>
       </c>
       <c r="C94">
-        <v>2354601</v>
+        <v>100908</v>
       </c>
       <c r="D94">
-        <v>1352297</v>
+        <v>3540724</v>
       </c>
       <c r="E94">
-        <v>5977751</v>
+        <v>5722519</v>
       </c>
       <c r="F94">
-        <v>315351</v>
+        <v>635849</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2277,16 +2277,16 @@
         <v>93</v>
       </c>
       <c r="C95">
-        <v>2054764</v>
+        <v>79740</v>
       </c>
       <c r="D95">
-        <v>1302400</v>
+        <v>3540236</v>
       </c>
       <c r="E95">
-        <v>6310114</v>
+        <v>5742020</v>
       </c>
       <c r="F95">
-        <v>332722</v>
+        <v>638004</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2297,16 +2297,16 @@
         <v>94</v>
       </c>
       <c r="C96">
-        <v>1777976</v>
+        <v>62667</v>
       </c>
       <c r="D96">
-        <v>1261125</v>
+        <v>3539848</v>
       </c>
       <c r="E96">
-        <v>6612543</v>
+        <v>5757744</v>
       </c>
       <c r="F96">
-        <v>348356</v>
+        <v>639741</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2317,16 +2317,16 @@
         <v>95</v>
       </c>
       <c r="C97">
-        <v>1528102</v>
+        <v>49342</v>
       </c>
       <c r="D97">
-        <v>1226691</v>
+        <v>3539503</v>
       </c>
       <c r="E97">
-        <v>6882634</v>
+        <v>5770075</v>
       </c>
       <c r="F97">
-        <v>362573</v>
+        <v>641080</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2337,16 +2337,16 @@
         <v>96</v>
       </c>
       <c r="C98">
-        <v>1305127</v>
+        <v>38766</v>
       </c>
       <c r="D98">
-        <v>1197691</v>
+        <v>3539262</v>
       </c>
       <c r="E98">
-        <v>7121990</v>
+        <v>5779788</v>
       </c>
       <c r="F98">
-        <v>375192</v>
+        <v>642184</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2357,16 +2357,16 @@
         <v>97</v>
       </c>
       <c r="C99">
-        <v>1109676</v>
+        <v>30549</v>
       </c>
       <c r="D99">
-        <v>1173651</v>
+        <v>3539068</v>
       </c>
       <c r="E99">
-        <v>7330442</v>
+        <v>5787359</v>
       </c>
       <c r="F99">
-        <v>386231</v>
+        <v>643024</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2377,16 +2377,16 @@
         <v>98</v>
       </c>
       <c r="C100">
-        <v>938938</v>
+        <v>23972</v>
       </c>
       <c r="D100">
-        <v>1153932</v>
+        <v>3538906</v>
       </c>
       <c r="E100">
-        <v>7511382</v>
+        <v>5793500</v>
       </c>
       <c r="F100">
-        <v>395748</v>
+        <v>643622</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2397,16 +2397,16 @@
         <v>99</v>
       </c>
       <c r="C101">
-        <v>791349</v>
+        <v>19002</v>
       </c>
       <c r="D101">
-        <v>1137565</v>
+        <v>3538797</v>
       </c>
       <c r="E101">
-        <v>7667265</v>
+        <v>5798041</v>
       </c>
       <c r="F101">
-        <v>403821</v>
+        <v>644160</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2417,16 +2417,16 @@
         <v>100</v>
       </c>
       <c r="C102">
-        <v>664427</v>
+        <v>15018</v>
       </c>
       <c r="D102">
-        <v>1123900</v>
+        <v>3538705</v>
       </c>
       <c r="E102">
-        <v>7800662</v>
+        <v>5801721</v>
       </c>
       <c r="F102">
-        <v>411011</v>
+        <v>644556</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2437,16 +2437,16 @@
         <v>101</v>
       </c>
       <c r="C103">
-        <v>556767</v>
+        <v>11839</v>
       </c>
       <c r="D103">
-        <v>1112627</v>
+        <v>3538653</v>
       </c>
       <c r="E103">
-        <v>7913743</v>
+        <v>5804603</v>
       </c>
       <c r="F103">
-        <v>416863</v>
+        <v>644905</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2457,16 +2457,16 @@
         <v>102</v>
       </c>
       <c r="C104">
-        <v>464854</v>
+        <v>9332</v>
       </c>
       <c r="D104">
-        <v>1103425</v>
+        <v>3538593</v>
       </c>
       <c r="E104">
-        <v>8009737</v>
+        <v>5806898</v>
       </c>
       <c r="F104">
-        <v>421984</v>
+        <v>645177</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -2477,16 +2477,16 @@
         <v>103</v>
       </c>
       <c r="C105">
-        <v>387412</v>
+        <v>7360</v>
       </c>
       <c r="D105">
-        <v>1095676</v>
+        <v>3538554</v>
       </c>
       <c r="E105">
-        <v>8090694</v>
+        <v>5808724</v>
       </c>
       <c r="F105">
-        <v>426218</v>
+        <v>645362</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2497,16 +2497,16 @@
         <v>104</v>
       </c>
       <c r="C106">
-        <v>322944</v>
+        <v>5821</v>
       </c>
       <c r="D106">
-        <v>1089234</v>
+        <v>3538502</v>
       </c>
       <c r="E106">
-        <v>8157932</v>
+        <v>5810154</v>
       </c>
       <c r="F106">
-        <v>429890</v>
+        <v>645523</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -2517,16 +2517,16 @@
         <v>105</v>
       </c>
       <c r="C107">
-        <v>268407</v>
+        <v>4611</v>
       </c>
       <c r="D107">
-        <v>1083890</v>
+        <v>3538472</v>
       </c>
       <c r="E107">
-        <v>8214897</v>
+        <v>5811283</v>
       </c>
       <c r="F107">
-        <v>432806</v>
+        <v>645634</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -2537,16 +2537,16 @@
         <v>106</v>
       </c>
       <c r="C108">
-        <v>222897</v>
+        <v>3639</v>
       </c>
       <c r="D108">
-        <v>1079503</v>
+        <v>3538445</v>
       </c>
       <c r="E108">
-        <v>8262356</v>
+        <v>5812196</v>
       </c>
       <c r="F108">
-        <v>435244</v>
+        <v>645720</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -2557,16 +2557,16 @@
         <v>107</v>
       </c>
       <c r="C109">
-        <v>185259</v>
+        <v>2924</v>
       </c>
       <c r="D109">
-        <v>1075866</v>
+        <v>3538426</v>
       </c>
       <c r="E109">
-        <v>8301543</v>
+        <v>5812847</v>
       </c>
       <c r="F109">
-        <v>437332</v>
+        <v>645803</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -2577,16 +2577,16 @@
         <v>108</v>
       </c>
       <c r="C110">
-        <v>153705</v>
+        <v>2313</v>
       </c>
       <c r="D110">
-        <v>1072986</v>
+        <v>3538411</v>
       </c>
       <c r="E110">
-        <v>8334265</v>
+        <v>5813402</v>
       </c>
       <c r="F110">
-        <v>439044</v>
+        <v>645874</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -2597,16 +2597,16 @@
         <v>109</v>
       </c>
       <c r="C111">
-        <v>127086</v>
+        <v>1836</v>
       </c>
       <c r="D111">
-        <v>1070605</v>
+        <v>3538400</v>
       </c>
       <c r="E111">
-        <v>8361792</v>
+        <v>5813855</v>
       </c>
       <c r="F111">
-        <v>440517</v>
+        <v>645909</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -2617,16 +2617,16 @@
         <v>110</v>
       </c>
       <c r="C112">
-        <v>105133</v>
+        <v>1460</v>
       </c>
       <c r="D112">
-        <v>1068518</v>
+        <v>3538388</v>
       </c>
       <c r="E112">
-        <v>8384575</v>
+        <v>5814195</v>
       </c>
       <c r="F112">
-        <v>441774</v>
+        <v>645957</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -2637,16 +2637,16 @@
         <v>111</v>
       </c>
       <c r="C113">
-        <v>87037</v>
+        <v>1120</v>
       </c>
       <c r="D113">
-        <v>1066895</v>
+        <v>3538383</v>
       </c>
       <c r="E113">
-        <v>8403284</v>
+        <v>5814511</v>
       </c>
       <c r="F113">
-        <v>442784</v>
+        <v>645986</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -2657,16 +2657,16 @@
         <v>112</v>
       </c>
       <c r="C114">
-        <v>72072</v>
+        <v>882</v>
       </c>
       <c r="D114">
-        <v>1065493</v>
+        <v>3538380</v>
       </c>
       <c r="E114">
-        <v>8418845</v>
+        <v>5814724</v>
       </c>
       <c r="F114">
-        <v>443590</v>
+        <v>646014</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -2677,16 +2677,16 @@
         <v>113</v>
       </c>
       <c r="C115">
-        <v>59564</v>
+        <v>695</v>
       </c>
       <c r="D115">
-        <v>1064336</v>
+        <v>3538373</v>
       </c>
       <c r="E115">
-        <v>8431837</v>
+        <v>5814896</v>
       </c>
       <c r="F115">
-        <v>444263</v>
+        <v>646036</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -2697,16 +2697,16 @@
         <v>114</v>
       </c>
       <c r="C116">
-        <v>49230</v>
+        <v>538</v>
       </c>
       <c r="D116">
-        <v>1063397</v>
+        <v>3538368</v>
       </c>
       <c r="E116">
-        <v>8442548</v>
+        <v>5815044</v>
       </c>
       <c r="F116">
-        <v>444825</v>
+        <v>646050</v>
       </c>
     </row>
     <row r="117" spans="1:6">
@@ -2717,16 +2717,16 @@
         <v>115</v>
       </c>
       <c r="C117">
-        <v>40785</v>
+        <v>430</v>
       </c>
       <c r="D117">
-        <v>1062640</v>
+        <v>3538367</v>
       </c>
       <c r="E117">
-        <v>8451286</v>
+        <v>5815140</v>
       </c>
       <c r="F117">
-        <v>445289</v>
+        <v>646063</v>
       </c>
     </row>
     <row r="118" spans="1:6">
@@ -2737,16 +2737,16 @@
         <v>116</v>
       </c>
       <c r="C118">
-        <v>33680</v>
+        <v>340</v>
       </c>
       <c r="D118">
-        <v>1061996</v>
+        <v>3538365</v>
       </c>
       <c r="E118">
-        <v>8458643</v>
+        <v>5815227</v>
       </c>
       <c r="F118">
-        <v>445681</v>
+        <v>646068</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -2757,16 +2757,16 @@
         <v>117</v>
       </c>
       <c r="C119">
-        <v>27758</v>
+        <v>290</v>
       </c>
       <c r="D119">
-        <v>1061476</v>
+        <v>3538363</v>
       </c>
       <c r="E119">
-        <v>8464753</v>
+        <v>5815276</v>
       </c>
       <c r="F119">
-        <v>446013</v>
+        <v>646071</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -2777,16 +2777,16 @@
         <v>118</v>
       </c>
       <c r="C120">
-        <v>22885</v>
+        <v>231</v>
       </c>
       <c r="D120">
-        <v>1061005</v>
+        <v>3538362</v>
       </c>
       <c r="E120">
-        <v>8469823</v>
+        <v>5815331</v>
       </c>
       <c r="F120">
-        <v>446287</v>
+        <v>646076</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -2797,16 +2797,16 @@
         <v>119</v>
       </c>
       <c r="C121">
-        <v>18851</v>
+        <v>192</v>
       </c>
       <c r="D121">
-        <v>1060652</v>
+        <v>3538362</v>
       </c>
       <c r="E121">
-        <v>8473997</v>
+        <v>5815363</v>
       </c>
       <c r="F121">
-        <v>446500</v>
+        <v>646083</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -2817,16 +2817,16 @@
         <v>120</v>
       </c>
       <c r="C122">
-        <v>15485</v>
+        <v>141</v>
       </c>
       <c r="D122">
-        <v>1060381</v>
+        <v>3538361</v>
       </c>
       <c r="E122">
-        <v>8477439</v>
+        <v>5815411</v>
       </c>
       <c r="F122">
-        <v>446695</v>
+        <v>646087</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -2837,16 +2837,16 @@
         <v>121</v>
       </c>
       <c r="C123">
-        <v>12859</v>
+        <v>112</v>
       </c>
       <c r="D123">
-        <v>1060127</v>
+        <v>3538360</v>
       </c>
       <c r="E123">
-        <v>8480158</v>
+        <v>5815438</v>
       </c>
       <c r="F123">
-        <v>446856</v>
+        <v>646090</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -2857,16 +2857,16 @@
         <v>122</v>
       </c>
       <c r="C124">
-        <v>10673</v>
+        <v>85</v>
       </c>
       <c r="D124">
-        <v>1059932</v>
+        <v>3538360</v>
       </c>
       <c r="E124">
-        <v>8482414</v>
+        <v>5815464</v>
       </c>
       <c r="F124">
-        <v>446981</v>
+        <v>646091</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -2877,16 +2877,16 @@
         <v>123</v>
       </c>
       <c r="C125">
-        <v>8764</v>
+        <v>66</v>
       </c>
       <c r="D125">
-        <v>1059754</v>
+        <v>3538360</v>
       </c>
       <c r="E125">
-        <v>8484395</v>
+        <v>5815479</v>
       </c>
       <c r="F125">
-        <v>447087</v>
+        <v>646095</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -2897,16 +2897,16 @@
         <v>124</v>
       </c>
       <c r="C126">
-        <v>7268</v>
+        <v>51</v>
       </c>
       <c r="D126">
-        <v>1059627</v>
+        <v>3538360</v>
       </c>
       <c r="E126">
-        <v>8485950</v>
+        <v>5815491</v>
       </c>
       <c r="F126">
-        <v>447155</v>
+        <v>646098</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -2917,16 +2917,16 @@
         <v>125</v>
       </c>
       <c r="C127">
-        <v>5971</v>
+        <v>40</v>
       </c>
       <c r="D127">
-        <v>1059522</v>
+        <v>3538360</v>
       </c>
       <c r="E127">
-        <v>8487288</v>
+        <v>5815501</v>
       </c>
       <c r="F127">
-        <v>447219</v>
+        <v>646099</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -2937,16 +2937,16 @@
         <v>126</v>
       </c>
       <c r="C128">
-        <v>4912</v>
+        <v>28</v>
       </c>
       <c r="D128">
-        <v>1059424</v>
+        <v>3538360</v>
       </c>
       <c r="E128">
-        <v>8488387</v>
+        <v>5815513</v>
       </c>
       <c r="F128">
-        <v>447277</v>
+        <v>646099</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -2957,16 +2957,16 @@
         <v>127</v>
       </c>
       <c r="C129">
-        <v>4055</v>
+        <v>23</v>
       </c>
       <c r="D129">
-        <v>1059342</v>
+        <v>3538360</v>
       </c>
       <c r="E129">
-        <v>8489286</v>
+        <v>5815517</v>
       </c>
       <c r="F129">
-        <v>447317</v>
+        <v>646100</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -2977,16 +2977,16 @@
         <v>128</v>
       </c>
       <c r="C130">
-        <v>3356</v>
+        <v>20</v>
       </c>
       <c r="D130">
-        <v>1059284</v>
+        <v>3538360</v>
       </c>
       <c r="E130">
-        <v>8490011</v>
+        <v>5815520</v>
       </c>
       <c r="F130">
-        <v>447349</v>
+        <v>646100</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -2997,16 +2997,16 @@
         <v>129</v>
       </c>
       <c r="C131">
-        <v>2766</v>
+        <v>13</v>
       </c>
       <c r="D131">
-        <v>1059230</v>
+        <v>3538360</v>
       </c>
       <c r="E131">
-        <v>8490620</v>
+        <v>5815527</v>
       </c>
       <c r="F131">
-        <v>447384</v>
+        <v>646100</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3017,16 +3017,16 @@
         <v>130</v>
       </c>
       <c r="C132">
-        <v>2298</v>
+        <v>8</v>
       </c>
       <c r="D132">
-        <v>1059178</v>
+        <v>3538360</v>
       </c>
       <c r="E132">
-        <v>8491116</v>
+        <v>5815531</v>
       </c>
       <c r="F132">
-        <v>447408</v>
+        <v>646101</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3037,16 +3037,16 @@
         <v>131</v>
       </c>
       <c r="C133">
-        <v>1861</v>
+        <v>7</v>
       </c>
       <c r="D133">
-        <v>1059144</v>
+        <v>3538360</v>
       </c>
       <c r="E133">
-        <v>8491559</v>
+        <v>5815532</v>
       </c>
       <c r="F133">
-        <v>447436</v>
+        <v>646101</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3057,16 +3057,16 @@
         <v>132</v>
       </c>
       <c r="C134">
-        <v>1534</v>
+        <v>5</v>
       </c>
       <c r="D134">
-        <v>1059118</v>
+        <v>3538360</v>
       </c>
       <c r="E134">
-        <v>8491890</v>
+        <v>5815534</v>
       </c>
       <c r="F134">
-        <v>447458</v>
+        <v>646101</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -3077,16 +3077,16 @@
         <v>133</v>
       </c>
       <c r="C135">
-        <v>1286</v>
+        <v>3</v>
       </c>
       <c r="D135">
-        <v>1059095</v>
+        <v>3538360</v>
       </c>
       <c r="E135">
-        <v>8492151</v>
+        <v>5815536</v>
       </c>
       <c r="F135">
-        <v>447468</v>
+        <v>646101</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -3097,16 +3097,16 @@
         <v>134</v>
       </c>
       <c r="C136">
-        <v>1045</v>
+        <v>2</v>
       </c>
       <c r="D136">
-        <v>1059082</v>
+        <v>3538360</v>
       </c>
       <c r="E136">
-        <v>8492396</v>
+        <v>5815537</v>
       </c>
       <c r="F136">
-        <v>447477</v>
+        <v>646101</v>
       </c>
     </row>
     <row r="137" spans="1:6">
@@ -3117,16 +3117,16 @@
         <v>135</v>
       </c>
       <c r="C137">
-        <v>866</v>
+        <v>2</v>
       </c>
       <c r="D137">
-        <v>1059066</v>
+        <v>3538360</v>
       </c>
       <c r="E137">
-        <v>8492583</v>
+        <v>5815537</v>
       </c>
       <c r="F137">
-        <v>447485</v>
+        <v>646101</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -3137,16 +3137,16 @@
         <v>136</v>
       </c>
       <c r="C138">
-        <v>704</v>
+        <v>1</v>
       </c>
       <c r="D138">
-        <v>1059050</v>
+        <v>3538360</v>
       </c>
       <c r="E138">
-        <v>8492753</v>
+        <v>5815537</v>
       </c>
       <c r="F138">
-        <v>447493</v>
+        <v>646102</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -3157,656 +3157,16 @@
         <v>137</v>
       </c>
       <c r="C139">
-        <v>586</v>
+        <v>0</v>
       </c>
       <c r="D139">
-        <v>1059041</v>
+        <v>3538360</v>
       </c>
       <c r="E139">
-        <v>8492876</v>
+        <v>5815538</v>
       </c>
       <c r="F139">
-        <v>447497</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6">
-      <c r="A140" s="1">
-        <v>138</v>
-      </c>
-      <c r="B140">
-        <v>138</v>
-      </c>
-      <c r="C140">
-        <v>486</v>
-      </c>
-      <c r="D140">
-        <v>1059036</v>
-      </c>
-      <c r="E140">
-        <v>8492975</v>
-      </c>
-      <c r="F140">
-        <v>447503</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6">
-      <c r="A141" s="1">
-        <v>139</v>
-      </c>
-      <c r="B141">
-        <v>139</v>
-      </c>
-      <c r="C141">
-        <v>393</v>
-      </c>
-      <c r="D141">
-        <v>1059031</v>
-      </c>
-      <c r="E141">
-        <v>8493072</v>
-      </c>
-      <c r="F141">
-        <v>447504</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6">
-      <c r="A142" s="1">
-        <v>140</v>
-      </c>
-      <c r="B142">
-        <v>140</v>
-      </c>
-      <c r="C142">
-        <v>316</v>
-      </c>
-      <c r="D142">
-        <v>1059026</v>
-      </c>
-      <c r="E142">
-        <v>8493151</v>
-      </c>
-      <c r="F142">
-        <v>447507</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6">
-      <c r="A143" s="1">
-        <v>141</v>
-      </c>
-      <c r="B143">
-        <v>141</v>
-      </c>
-      <c r="C143">
-        <v>264</v>
-      </c>
-      <c r="D143">
-        <v>1059020</v>
-      </c>
-      <c r="E143">
-        <v>8493205</v>
-      </c>
-      <c r="F143">
-        <v>447511</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6">
-      <c r="A144" s="1">
-        <v>142</v>
-      </c>
-      <c r="B144">
-        <v>142</v>
-      </c>
-      <c r="C144">
-        <v>216</v>
-      </c>
-      <c r="D144">
-        <v>1059014</v>
-      </c>
-      <c r="E144">
-        <v>8493255</v>
-      </c>
-      <c r="F144">
-        <v>447515</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6">
-      <c r="A145" s="1">
-        <v>143</v>
-      </c>
-      <c r="B145">
-        <v>143</v>
-      </c>
-      <c r="C145">
-        <v>168</v>
-      </c>
-      <c r="D145">
-        <v>1059010</v>
-      </c>
-      <c r="E145">
-        <v>8493302</v>
-      </c>
-      <c r="F145">
-        <v>447520</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6">
-      <c r="A146" s="1">
-        <v>144</v>
-      </c>
-      <c r="B146">
-        <v>144</v>
-      </c>
-      <c r="C146">
-        <v>138</v>
-      </c>
-      <c r="D146">
-        <v>1059006</v>
-      </c>
-      <c r="E146">
-        <v>8493336</v>
-      </c>
-      <c r="F146">
-        <v>447520</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6">
-      <c r="A147" s="1">
-        <v>145</v>
-      </c>
-      <c r="B147">
-        <v>145</v>
-      </c>
-      <c r="C147">
-        <v>115</v>
-      </c>
-      <c r="D147">
-        <v>1059003</v>
-      </c>
-      <c r="E147">
-        <v>8493360</v>
-      </c>
-      <c r="F147">
-        <v>447522</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6">
-      <c r="A148" s="1">
-        <v>146</v>
-      </c>
-      <c r="B148">
-        <v>146</v>
-      </c>
-      <c r="C148">
-        <v>94</v>
-      </c>
-      <c r="D148">
-        <v>1059001</v>
-      </c>
-      <c r="E148">
-        <v>8493382</v>
-      </c>
-      <c r="F148">
-        <v>447523</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6">
-      <c r="A149" s="1">
-        <v>147</v>
-      </c>
-      <c r="B149">
-        <v>147</v>
-      </c>
-      <c r="C149">
-        <v>82</v>
-      </c>
-      <c r="D149">
-        <v>1059000</v>
-      </c>
-      <c r="E149">
-        <v>8493395</v>
-      </c>
-      <c r="F149">
-        <v>447523</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6">
-      <c r="A150" s="1">
-        <v>148</v>
-      </c>
-      <c r="B150">
-        <v>148</v>
-      </c>
-      <c r="C150">
-        <v>69</v>
-      </c>
-      <c r="D150">
-        <v>1058997</v>
-      </c>
-      <c r="E150">
-        <v>8493411</v>
-      </c>
-      <c r="F150">
-        <v>447523</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6">
-      <c r="A151" s="1">
-        <v>149</v>
-      </c>
-      <c r="B151">
-        <v>149</v>
-      </c>
-      <c r="C151">
-        <v>56</v>
-      </c>
-      <c r="D151">
-        <v>1058994</v>
-      </c>
-      <c r="E151">
-        <v>8493426</v>
-      </c>
-      <c r="F151">
-        <v>447524</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6">
-      <c r="A152" s="1">
-        <v>150</v>
-      </c>
-      <c r="B152">
-        <v>150</v>
-      </c>
-      <c r="C152">
-        <v>48</v>
-      </c>
-      <c r="D152">
-        <v>1058993</v>
-      </c>
-      <c r="E152">
-        <v>8493434</v>
-      </c>
-      <c r="F152">
-        <v>447525</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6">
-      <c r="A153" s="1">
-        <v>151</v>
-      </c>
-      <c r="B153">
-        <v>151</v>
-      </c>
-      <c r="C153">
-        <v>45</v>
-      </c>
-      <c r="D153">
-        <v>1058991</v>
-      </c>
-      <c r="E153">
-        <v>8493439</v>
-      </c>
-      <c r="F153">
-        <v>447525</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6">
-      <c r="A154" s="1">
-        <v>152</v>
-      </c>
-      <c r="B154">
-        <v>152</v>
-      </c>
-      <c r="C154">
-        <v>40</v>
-      </c>
-      <c r="D154">
-        <v>1058991</v>
-      </c>
-      <c r="E154">
-        <v>8493443</v>
-      </c>
-      <c r="F154">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6">
-      <c r="A155" s="1">
-        <v>153</v>
-      </c>
-      <c r="B155">
-        <v>153</v>
-      </c>
-      <c r="C155">
-        <v>35</v>
-      </c>
-      <c r="D155">
-        <v>1058991</v>
-      </c>
-      <c r="E155">
-        <v>8493448</v>
-      </c>
-      <c r="F155">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6">
-      <c r="A156" s="1">
-        <v>154</v>
-      </c>
-      <c r="B156">
-        <v>154</v>
-      </c>
-      <c r="C156">
-        <v>31</v>
-      </c>
-      <c r="D156">
-        <v>1058989</v>
-      </c>
-      <c r="E156">
-        <v>8493454</v>
-      </c>
-      <c r="F156">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6">
-      <c r="A157" s="1">
-        <v>155</v>
-      </c>
-      <c r="B157">
-        <v>155</v>
-      </c>
-      <c r="C157">
-        <v>25</v>
-      </c>
-      <c r="D157">
-        <v>1058989</v>
-      </c>
-      <c r="E157">
-        <v>8493460</v>
-      </c>
-      <c r="F157">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6">
-      <c r="A158" s="1">
-        <v>156</v>
-      </c>
-      <c r="B158">
-        <v>156</v>
-      </c>
-      <c r="C158">
-        <v>22</v>
-      </c>
-      <c r="D158">
-        <v>1058988</v>
-      </c>
-      <c r="E158">
-        <v>8493464</v>
-      </c>
-      <c r="F158">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6">
-      <c r="A159" s="1">
-        <v>157</v>
-      </c>
-      <c r="B159">
-        <v>157</v>
-      </c>
-      <c r="C159">
-        <v>18</v>
-      </c>
-      <c r="D159">
-        <v>1058988</v>
-      </c>
-      <c r="E159">
-        <v>8493468</v>
-      </c>
-      <c r="F159">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6">
-      <c r="A160" s="1">
-        <v>158</v>
-      </c>
-      <c r="B160">
-        <v>158</v>
-      </c>
-      <c r="C160">
-        <v>15</v>
-      </c>
-      <c r="D160">
-        <v>1058988</v>
-      </c>
-      <c r="E160">
-        <v>8493471</v>
-      </c>
-      <c r="F160">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6">
-      <c r="A161" s="1">
-        <v>159</v>
-      </c>
-      <c r="B161">
-        <v>159</v>
-      </c>
-      <c r="C161">
-        <v>13</v>
-      </c>
-      <c r="D161">
-        <v>1058988</v>
-      </c>
-      <c r="E161">
-        <v>8493473</v>
-      </c>
-      <c r="F161">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6">
-      <c r="A162" s="1">
-        <v>160</v>
-      </c>
-      <c r="B162">
-        <v>160</v>
-      </c>
-      <c r="C162">
-        <v>12</v>
-      </c>
-      <c r="D162">
-        <v>1058988</v>
-      </c>
-      <c r="E162">
-        <v>8493474</v>
-      </c>
-      <c r="F162">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6">
-      <c r="A163" s="1">
-        <v>161</v>
-      </c>
-      <c r="B163">
-        <v>161</v>
-      </c>
-      <c r="C163">
-        <v>9</v>
-      </c>
-      <c r="D163">
-        <v>1058988</v>
-      </c>
-      <c r="E163">
-        <v>8493477</v>
-      </c>
-      <c r="F163">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6">
-      <c r="A164" s="1">
-        <v>162</v>
-      </c>
-      <c r="B164">
-        <v>162</v>
-      </c>
-      <c r="C164">
-        <v>6</v>
-      </c>
-      <c r="D164">
-        <v>1058988</v>
-      </c>
-      <c r="E164">
-        <v>8493480</v>
-      </c>
-      <c r="F164">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6">
-      <c r="A165" s="1">
-        <v>163</v>
-      </c>
-      <c r="B165">
-        <v>163</v>
-      </c>
-      <c r="C165">
-        <v>5</v>
-      </c>
-      <c r="D165">
-        <v>1058988</v>
-      </c>
-      <c r="E165">
-        <v>8493481</v>
-      </c>
-      <c r="F165">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6">
-      <c r="A166" s="1">
-        <v>164</v>
-      </c>
-      <c r="B166">
-        <v>164</v>
-      </c>
-      <c r="C166">
-        <v>3</v>
-      </c>
-      <c r="D166">
-        <v>1058988</v>
-      </c>
-      <c r="E166">
-        <v>8493483</v>
-      </c>
-      <c r="F166">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6">
-      <c r="A167" s="1">
-        <v>165</v>
-      </c>
-      <c r="B167">
-        <v>165</v>
-      </c>
-      <c r="C167">
-        <v>3</v>
-      </c>
-      <c r="D167">
-        <v>1058988</v>
-      </c>
-      <c r="E167">
-        <v>8493483</v>
-      </c>
-      <c r="F167">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6">
-      <c r="A168" s="1">
-        <v>166</v>
-      </c>
-      <c r="B168">
-        <v>166</v>
-      </c>
-      <c r="C168">
-        <v>3</v>
-      </c>
-      <c r="D168">
-        <v>1058988</v>
-      </c>
-      <c r="E168">
-        <v>8493483</v>
-      </c>
-      <c r="F168">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6">
-      <c r="A169" s="1">
-        <v>167</v>
-      </c>
-      <c r="B169">
-        <v>167</v>
-      </c>
-      <c r="C169">
-        <v>1</v>
-      </c>
-      <c r="D169">
-        <v>1058988</v>
-      </c>
-      <c r="E169">
-        <v>8493485</v>
-      </c>
-      <c r="F169">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6">
-      <c r="A170" s="1">
-        <v>168</v>
-      </c>
-      <c r="B170">
-        <v>168</v>
-      </c>
-      <c r="C170">
-        <v>1</v>
-      </c>
-      <c r="D170">
-        <v>1058988</v>
-      </c>
-      <c r="E170">
-        <v>8493485</v>
-      </c>
-      <c r="F170">
-        <v>447526</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6">
-      <c r="A171" s="1">
-        <v>169</v>
-      </c>
-      <c r="B171">
-        <v>169</v>
-      </c>
-      <c r="C171">
-        <v>0</v>
-      </c>
-      <c r="D171">
-        <v>1058988</v>
-      </c>
-      <c r="E171">
-        <v>8493486</v>
-      </c>
-      <c r="F171">
-        <v>447526</v>
+        <v>646102</v>
       </c>
     </row>
   </sheetData>

</xml_diff>